<commit_message>
Refactored the code a little bit
</commit_message>
<xml_diff>
--- a/dbc_parser/dbc_output_new.xlsx
+++ b/dbc_parser/dbc_output_new.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="CANFD2 messages" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CANFD2 signals" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CANFD2 enums" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample DBC messages" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sample DBC signals" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sample DBC enums" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>